<commit_message>
add time to atomic block
</commit_message>
<xml_diff>
--- a/requirements/next_steps.xlsx
+++ b/requirements/next_steps.xlsx
@@ -206,7 +206,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -225,6 +225,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -238,7 +244,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -258,6 +264,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Звичайний" xfId="0" builtinId="0"/>
@@ -561,8 +568,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -736,7 +743,7 @@
       <c r="A17" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="7" t="s">
         <v>43</v>
       </c>
     </row>
@@ -744,7 +751,7 @@
       <c r="A18" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="7" t="s">
         <v>43</v>
       </c>
     </row>

</xml_diff>